<commit_message>
cập nhật 6/1/2026 : sửa edit phiếu nhập xuất và sửa product
</commit_message>
<xml_diff>
--- a/backend/templates/product_template.xlsx
+++ b/backend/templates/product_template.xlsx
@@ -1,24 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F0CC1E-944D-4F3B-9508-3AAE3F2C79E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Template" state="visible" r:id="rId4"/>
+    <sheet name="Template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Tên sản phẩm</t>
   </si>
   <si>
-    <t>Mô tả</t>
-  </si>
-  <si>
     <t>Mã SKU</t>
   </si>
   <si>
@@ -31,28 +43,28 @@
     <t>Tồn kho</t>
   </si>
   <si>
-    <t>Tồn kho tối thiểu</t>
-  </si>
-  <si>
-    <t>Tồn kho tối đa</t>
-  </si>
-  <si>
     <t>Đơn vị</t>
   </si>
   <si>
-    <t>Trạng thái</t>
-  </si>
-  <si>
     <t>Nhà cung cấp</t>
   </si>
   <si>
+    <t>Số lô</t>
+  </si>
+  <si>
+    <t>Hạn sử dụng</t>
+  </si>
+  <si>
+    <t>Số chứng từ</t>
+  </si>
+  <si>
+    <t>Ngày chứng từ</t>
+  </si>
+  <si>
     <t>Nhóm sản phẩm</t>
   </si>
   <si>
-    <t>Coca Cola 330ml</t>
-  </si>
-  <si>
-    <t>Nước ngọt</t>
+    <t>Coca Cola Lon 330ml</t>
   </si>
   <si>
     <t>SP000001</t>
@@ -61,10 +73,19 @@
     <t>Lon</t>
   </si>
   <si>
-    <t>Đang kinh doanh</t>
-  </si>
-  <si>
-    <t>Coca Cola VN</t>
+    <t>Công ty CocaCola</t>
+  </si>
+  <si>
+    <t>L01</t>
+  </si>
+  <si>
+    <t>2026-12-31</t>
+  </si>
+  <si>
+    <t>NK001</t>
+  </si>
+  <si>
+    <t>2025-01-01</t>
   </si>
   <si>
     <t>Đồ uống</t>
@@ -73,48 +94,55 @@
     <t>Bánh mì sandwich</t>
   </si>
   <si>
-    <t>Bánh mì kẹp</t>
-  </si>
-  <si>
     <t>SP000002</t>
   </si>
   <si>
     <t>Cái</t>
   </si>
   <si>
-    <t>Bánh mì ABC</t>
-  </si>
-  <si>
-    <t>Thực phẩm</t>
+    <t>Bánh Mỳ ABC</t>
+  </si>
+  <si>
+    <t>L02</t>
+  </si>
+  <si>
+    <t>NK002</t>
+  </si>
+  <si>
+    <t>2025-01-02</t>
+  </si>
+  <si>
+    <t>Thực Phẩm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
       <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF4472C4"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -130,14 +158,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -470,14 +500,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L3"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="12" width="18" customWidth="1"/>
+    <col min="1" max="1" width="25.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="12.81640625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="10.81640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.81640625" style="1" customWidth="1"/>
+    <col min="8" max="11" width="15.81640625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -516,83 +557,87 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1">
+        <v>10000</v>
+      </c>
+      <c r="D2" s="1">
+        <v>8000</v>
+      </c>
+      <c r="E2" s="1">
+        <v>100</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2">
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1">
+        <v>15000</v>
+      </c>
+      <c r="D3" s="1">
         <v>10000</v>
       </c>
-      <c r="E2">
-        <v>8000</v>
-      </c>
-      <c r="F2">
-        <v>100</v>
-      </c>
-      <c r="G2">
-        <v>20</v>
-      </c>
-      <c r="H2">
-        <v>500</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="E3" s="1">
+        <v>50</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3">
-        <v>15000</v>
-      </c>
-      <c r="E3">
-        <v>10000</v>
-      </c>
-      <c r="F3">
-        <v>50</v>
-      </c>
-      <c r="G3">
-        <v>10</v>
-      </c>
-      <c r="H3">
-        <v>200</v>
-      </c>
-      <c r="I3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" t="s">
-        <v>24</v>
+      <c r="J3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1:L1 B3:E3 A2:B2 E2:L2" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>